<commit_message>
adiciona planilha do segundo bimestre
</commit_message>
<xml_diff>
--- a/data-prep/planilhas-bimestral-2022-1bim.xlsx
+++ b/data-prep/planilhas-bimestral-2022-1bim.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/bimestral/data-prep/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\github\bimestral\data-prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2E9AB8-850A-924E-BFA5-F1A785BE6D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B102A3-32C4-4B03-81A8-A4D09A6B0800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27400" yWindow="2840" windowWidth="25600" windowHeight="14180" tabRatio="812" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="812" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="50" r:id="rId1"/>
@@ -3284,37 +3284,37 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="31">
-    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;R$ &quot;#,##0.00_);[Red]\(&quot;R$ &quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="169" formatCode="#.##000"/>
-    <numFmt numFmtId="170" formatCode="%#,#00"/>
-    <numFmt numFmtId="171" formatCode="#,#00"/>
-    <numFmt numFmtId="172" formatCode="#.##0,"/>
-    <numFmt numFmtId="173" formatCode="\$#,"/>
-    <numFmt numFmtId="174" formatCode="General_)"/>
-    <numFmt numFmtId="175" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="#,##0.0_);\(#,##0.0\)"/>
-    <numFmt numFmtId="178" formatCode="0.0"/>
-    <numFmt numFmtId="179" formatCode="0.0%"/>
-    <numFmt numFmtId="180" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
-    <numFmt numFmtId="181" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="182" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="183" formatCode="#,##0_ ;\-#,##0\ "/>
-    <numFmt numFmtId="184" formatCode="#,##0\ &quot;Esc.&quot;;\-#,##0\ &quot;Esc.&quot;"/>
-    <numFmt numFmtId="185" formatCode="#,##0.00\ &quot;Esc.&quot;;\-#,##0.00\ &quot;Esc.&quot;"/>
-    <numFmt numFmtId="186" formatCode="#,##0.00\ &quot;Esc.&quot;;[Red]\-#,##0.00\ &quot;Esc.&quot;"/>
-    <numFmt numFmtId="187" formatCode="#,##0\ \ "/>
-    <numFmt numFmtId="188" formatCode="#,##0.##"/>
-    <numFmt numFmtId="189" formatCode="0.000000000000"/>
-    <numFmt numFmtId="190" formatCode="#,##0.#"/>
-    <numFmt numFmtId="191" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="192" formatCode="#\ ###\ ##0.00_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$ &quot;#,##0.00_);[Red]\(&quot;R$ &quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="169" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="170" formatCode="#.##000"/>
+    <numFmt numFmtId="171" formatCode="%#,#00"/>
+    <numFmt numFmtId="172" formatCode="#,#00"/>
+    <numFmt numFmtId="173" formatCode="#.##0,"/>
+    <numFmt numFmtId="174" formatCode="\$#,"/>
+    <numFmt numFmtId="175" formatCode="General_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="#,##0.0_);\(#,##0.0\)"/>
+    <numFmt numFmtId="179" formatCode="0.0"/>
+    <numFmt numFmtId="180" formatCode="0.0%"/>
+    <numFmt numFmtId="181" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="182" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="183" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="184" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="185" formatCode="#,##0\ &quot;Esc.&quot;;\-#,##0\ &quot;Esc.&quot;"/>
+    <numFmt numFmtId="186" formatCode="#,##0.00\ &quot;Esc.&quot;;\-#,##0.00\ &quot;Esc.&quot;"/>
+    <numFmt numFmtId="187" formatCode="#,##0.00\ &quot;Esc.&quot;;[Red]\-#,##0.00\ &quot;Esc.&quot;"/>
+    <numFmt numFmtId="188" formatCode="#,##0\ \ "/>
+    <numFmt numFmtId="189" formatCode="#,##0.##"/>
+    <numFmt numFmtId="190" formatCode="0.000000000000"/>
+    <numFmt numFmtId="191" formatCode="#,##0.#"/>
+    <numFmt numFmtId="192" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="193" formatCode="#\ ###\ ##0.00_)"/>
   </numFmts>
   <fonts count="132">
     <font>
@@ -5106,18 +5106,18 @@
     <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="174" fontId="60" fillId="0" borderId="1"/>
-    <xf numFmtId="174" fontId="39" fillId="0" borderId="1"/>
-    <xf numFmtId="174" fontId="25" fillId="0" borderId="0">
+    <xf numFmtId="175" fontId="60" fillId="0" borderId="1"/>
+    <xf numFmtId="175" fontId="39" fillId="0" borderId="1"/>
+    <xf numFmtId="175" fontId="25" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="174" fontId="26" fillId="0" borderId="0">
+    <xf numFmtId="175" fontId="26" fillId="0" borderId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="58" fillId="0" borderId="0">
+    <xf numFmtId="175" fontId="58" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="174" fontId="26" fillId="0" borderId="0">
+    <xf numFmtId="175" fontId="26" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5142,7 +5142,7 @@
     <xf numFmtId="0" fontId="35" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="40" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5159,11 +5159,11 @@
     <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="181" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="5">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="20" fillId="0" borderId="0">
+    <xf numFmtId="172" fontId="20" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" applyNumberFormat="0">
@@ -5181,7 +5181,7 @@
     <xf numFmtId="0" fontId="63" fillId="0" borderId="7">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="20" fillId="0" borderId="0">
+    <xf numFmtId="174" fontId="20" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5195,16 +5195,16 @@
     <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="73" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="10" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="20" fillId="0" borderId="0">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="186" fontId="73" fillId="0" borderId="0">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="170" fontId="20" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="185" fontId="73" fillId="0" borderId="0">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="184" fontId="73" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5217,20 +5217,20 @@
     <xf numFmtId="38" fontId="59" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="38" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="38" fontId="23" fillId="0" borderId="10"/>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="169" fontId="19" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="74" fillId="0" borderId="0">
+    <xf numFmtId="188" fontId="74" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="69" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="69" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="76" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="69" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="69" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="76" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0">
@@ -5244,13 +5244,13 @@
     <xf numFmtId="2" fontId="24" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="186" fontId="73" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="73" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="24" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="186" fontId="73" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="73" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="20" fillId="0" borderId="14">
@@ -5259,18 +5259,18 @@
     <xf numFmtId="3" fontId="20" fillId="0" borderId="14">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0">
+    <xf numFmtId="170" fontId="20" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="172" fontId="20" fillId="0" borderId="0">
+    <xf numFmtId="173" fontId="20" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="67" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="67" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="69" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="73" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="76" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5282,21 +5282,30 @@
     <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="103" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="103" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="103" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="191" fontId="103" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="192" fontId="103" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="191" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="192" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="186" fontId="19" fillId="0" borderId="0">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="186" fontId="19" fillId="0" borderId="0">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="186" fontId="19" fillId="0" borderId="0">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="185" fontId="19" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
@@ -5304,15 +5313,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="185" fontId="19" fillId="0" borderId="0">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="184" fontId="19" fillId="0" borderId="0">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="184" fontId="19" fillId="0" borderId="0">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="184" fontId="19" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5324,7 +5324,7 @@
     <xf numFmtId="38" fontId="104" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="38" fontId="104" fillId="0" borderId="10"/>
     <xf numFmtId="38" fontId="23" fillId="0" borderId="10"/>
-    <xf numFmtId="192" fontId="23" fillId="0" borderId="0">
+    <xf numFmtId="193" fontId="23" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5333,22 +5333,22 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="19" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="186" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="19" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="186" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="19" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="186" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="19" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="186" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="19" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="186" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="187" fontId="19" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5357,20 +5357,20 @@
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="106" fillId="0" borderId="0">
+    <xf numFmtId="169" fontId="106" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="43" fontId="106" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="180" fontId="115" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="191" fontId="115" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="181" fontId="115" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="192" fontId="115" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="115" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="115" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="115" fillId="0" borderId="0">
+    <xf numFmtId="169" fontId="115" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="43" fontId="115" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5382,7 +5382,7 @@
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="116" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -5391,7 +5391,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -5406,13 +5406,13 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="52" fillId="0" borderId="0" xfId="89" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="89" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="48" fillId="0" borderId="0" xfId="89" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="48" fillId="0" borderId="0" xfId="89" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="48" fillId="0" borderId="5" xfId="89" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="48" fillId="0" borderId="5" xfId="89" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5425,15 +5425,15 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="50" fillId="0" borderId="5" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="50" fillId="0" borderId="5" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="5" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="5" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -5442,22 +5442,22 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="51" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="51" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="51" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="51" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
     </xf>
@@ -5465,82 +5465,82 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="0" borderId="0" xfId="91" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="51" fillId="0" borderId="0" xfId="91" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="168" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="48" fillId="0" borderId="0" xfId="111" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="48" fillId="0" borderId="0" xfId="75" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="179" fontId="48" fillId="0" borderId="0" xfId="75" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="48" fillId="0" borderId="0" xfId="75" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="66" fillId="25" borderId="16" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="66" fillId="25" borderId="16" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="66" fillId="25" borderId="27" xfId="89" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="66" fillId="25" borderId="27" xfId="89" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="66" fillId="25" borderId="28" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="66" fillId="25" borderId="28" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="66" fillId="25" borderId="17" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="66" fillId="25" borderId="17" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="50" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="50" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="65" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="65" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="8" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5574,14 +5574,14 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="66" applyFont="1"/>
-    <xf numFmtId="166" fontId="67" fillId="0" borderId="0" xfId="112"/>
-    <xf numFmtId="166" fontId="67" fillId="0" borderId="0" xfId="112" applyFill="1"/>
+    <xf numFmtId="167" fontId="67" fillId="0" borderId="0" xfId="112"/>
+    <xf numFmtId="167" fontId="67" fillId="0" borderId="0" xfId="112" applyFill="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="66" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5603,43 +5603,43 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="66" applyFont="1"/>
-    <xf numFmtId="166" fontId="85" fillId="0" borderId="0" xfId="112" applyFont="1"/>
+    <xf numFmtId="167" fontId="85" fillId="0" borderId="0" xfId="112" applyFont="1"/>
     <xf numFmtId="3" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="52" fillId="29" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="52" fillId="29" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="50" fillId="0" borderId="5" xfId="92" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="50" fillId="0" borderId="5" xfId="92" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="5" xfId="92" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="5" xfId="92" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="66" fillId="25" borderId="17" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="66" fillId="25" borderId="17" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="52" fillId="0" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="52" fillId="0" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="48" fillId="0" borderId="0" xfId="113" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="48" fillId="0" borderId="0" xfId="113" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="52" fillId="0" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="24" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="51" fillId="24" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -5649,7 +5649,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="66" fillId="25" borderId="16" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="66" fillId="25" borderId="16" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5672,21 +5672,21 @@
     <xf numFmtId="2" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="85" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="85" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="66" fillId="25" borderId="33" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="66" fillId="25" borderId="33" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="66" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="82" fillId="28" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="48" fillId="0" borderId="0" xfId="111" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -5694,22 +5694,22 @@
     <xf numFmtId="3" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="65" fillId="0" borderId="5" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="65" fillId="0" borderId="5" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="65" fillId="0" borderId="5" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="65" fillId="0" borderId="5" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="111" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="52" fillId="0" borderId="0" xfId="111" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="50" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="50" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -5719,7 +5719,7 @@
     <xf numFmtId="9" fontId="80" fillId="27" borderId="30" xfId="75" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="52" fillId="0" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="52" fillId="0" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -5732,44 +5732,44 @@
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
-    <xf numFmtId="167" fontId="55" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="55" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="48" fillId="0" borderId="0" xfId="117" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="88" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="88" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="168" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="84" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="168" fontId="84" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="168" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="51" fillId="24" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="51" fillId="24" borderId="0" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="51" fillId="0" borderId="0" xfId="91" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="51" fillId="0" borderId="0" xfId="91" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="51" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="51" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="48" fillId="0" borderId="0" xfId="75" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -5779,18 +5779,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="61" applyFont="1"/>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="61" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="61" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="61" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="93" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="93" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -5804,53 +5804,53 @@
     <xf numFmtId="4" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="29" borderId="0" xfId="93" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="29" borderId="0" xfId="93" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="29" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="29" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="93" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="93" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="93" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="93" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="89" fillId="29" borderId="0" xfId="61" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="89" fillId="29" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="29" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="89" fillId="29" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -5864,35 +5864,35 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="29" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="29" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5900,7 +5900,7 @@
     <xf numFmtId="0" fontId="84" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="52" fillId="29" borderId="36" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="52" fillId="29" borderId="36" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -5908,7 +5908,7 @@
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="120" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="188" fontId="79" fillId="0" borderId="0" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="79" fillId="0" borderId="0" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="94" fillId="27" borderId="31" xfId="120" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5924,17 +5924,17 @@
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="120" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="79" fillId="0" borderId="0" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="79" fillId="0" borderId="0" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="120" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="97" fillId="0" borderId="0" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="97" fillId="0" borderId="0" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="52" fillId="0" borderId="0" xfId="111" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5943,7 +5943,7 @@
     <xf numFmtId="4" fontId="48" fillId="0" borderId="0" xfId="111" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="189" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5956,7 +5956,7 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="79" fillId="0" borderId="0" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="79" fillId="0" borderId="0" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="120" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5975,50 +5975,50 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="120" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="190" fontId="98" fillId="0" borderId="5" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="191" fontId="98" fillId="0" borderId="5" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="101" fillId="25" borderId="16" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="101" fillId="25" borderId="16" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="101" fillId="25" borderId="28" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="101" fillId="25" borderId="28" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="101" fillId="25" borderId="29" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="101" fillId="25" borderId="29" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="86" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="86" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="86" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="86" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="3"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="102" fillId="28" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="102" fillId="28" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="102" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="102" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="102" fillId="28" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="102" fillId="28" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="102" fillId="28" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="102" fillId="28" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="102" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="102" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="102" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="102" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -6032,7 +6032,7 @@
     <xf numFmtId="0" fontId="98" fillId="0" borderId="5" xfId="120" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="52" fillId="0" borderId="0" xfId="91" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="52" fillId="0" borderId="0" xfId="91" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="111" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6043,10 +6043,10 @@
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="111" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="175" fontId="53" fillId="0" borderId="0" xfId="90" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="53" fillId="0" borderId="0" xfId="90" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="66" fillId="25" borderId="34" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="66" fillId="25" borderId="34" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -6054,7 +6054,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="22" xfId="111" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
@@ -6065,33 +6065,33 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="86" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="86" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="109" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="109" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="177" fontId="109" fillId="29" borderId="36" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="109" fillId="29" borderId="36" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="110" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="168" fontId="110" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6102,17 +6102,17 @@
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="181" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="181" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="181" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="182" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="182" fontId="84" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="182" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="97" fillId="0" borderId="0" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="97" fillId="0" borderId="0" xfId="120" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="61" applyFont="1"/>
@@ -6127,7 +6127,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="79" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="79" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="53" fillId="0" borderId="0" xfId="111" applyFont="1" applyAlignment="1">
@@ -6142,7 +6142,7 @@
     <xf numFmtId="0" fontId="48" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="53" fillId="0" borderId="18" xfId="90" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="53" fillId="0" borderId="18" xfId="90" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="40" xfId="137" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6150,12 +6150,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="89" fillId="0" borderId="40" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="40" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="40" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="40" xfId="137" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="61" applyFont="1"/>
@@ -6180,7 +6180,7 @@
     <xf numFmtId="0" fontId="81" fillId="29" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="81" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="81" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="80" fillId="27" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6192,10 +6192,10 @@
     <xf numFmtId="0" fontId="81" fillId="29" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="167" fontId="81" fillId="29" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="81" fillId="29" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="175" fontId="53" fillId="27" borderId="18" xfId="90" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="53" fillId="27" borderId="18" xfId="90" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="114" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -6210,17 +6210,17 @@
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="167" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="167" fontId="102" fillId="29" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="102" fillId="29" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="102" fillId="29" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="102" fillId="29" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -6245,8 +6245,8 @@
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="120" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="201" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="201" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="182" fontId="3" fillId="0" borderId="0" xfId="201" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="182" fontId="3" fillId="0" borderId="0" xfId="201" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="48" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -6256,15 +6256,15 @@
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="101" fillId="25" borderId="44" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="101" fillId="25" borderId="44" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="52" fillId="29" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="52" fillId="29" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="109" fillId="29" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="109" fillId="29" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -6304,34 +6304,34 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="137" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="51" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="51" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="51" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="51" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="137" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
     </xf>
-    <xf numFmtId="167" fontId="53" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="53" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="53" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="53" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="53" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="53" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="53" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="53" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="32" borderId="0" xfId="137" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6340,17 +6340,17 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="137" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
     </xf>
-    <xf numFmtId="167" fontId="53" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="53" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="137" applyFill="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="137" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="137" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="137" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="137" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="5"/>
     </xf>
@@ -6360,68 +6360,68 @@
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="137" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="5"/>
     </xf>
-    <xf numFmtId="167" fontId="109" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="109" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="109" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="109" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="109" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="109" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="109" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="109" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="137" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="7"/>
     </xf>
-    <xf numFmtId="167" fontId="120" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="120" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="120" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="120" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="120" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="120" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="120" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="120" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="196" applyFont="1"/>
-    <xf numFmtId="167" fontId="119" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="196" applyFont="1"/>
+    <xf numFmtId="168" fontId="119" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="53" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="53" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="137" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="137" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="118" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="118" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="118" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="118" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="118" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="118" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="118" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="118" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" xfId="137" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="51" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="51" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="51" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="51" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="51" fillId="32" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="196" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="196" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="137" applyAlignment="1">
@@ -6430,50 +6430,50 @@
     <xf numFmtId="0" fontId="118" fillId="0" borderId="39" xfId="137" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="118" fillId="0" borderId="48" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="118" fillId="0" borderId="48" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="118" fillId="0" borderId="39" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="118" fillId="0" borderId="39" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="118" fillId="0" borderId="39" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="118" fillId="0" borderId="39" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="118" fillId="32" borderId="39" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="118" fillId="32" borderId="39" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="38" xfId="137" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="109" fillId="0" borderId="38" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="109" fillId="0" borderId="38" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="137" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="120" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="120" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="121" fillId="0" borderId="21" xfId="137" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="53" fillId="0" borderId="23" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="53" fillId="0" borderId="0" xfId="196" applyFont="1"/>
+    <xf numFmtId="168" fontId="53" fillId="0" borderId="23" xfId="137" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="53" fillId="0" borderId="0" xfId="196" applyFont="1"/>
     <xf numFmtId="43" fontId="53" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="137" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="5"/>
     </xf>
-    <xf numFmtId="167" fontId="109" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="109" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="137" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="7"/>
     </xf>
-    <xf numFmtId="167" fontId="120" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="120" fillId="0" borderId="47" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="137" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
     </xf>
-    <xf numFmtId="167" fontId="53" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="53" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="125" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="79" fillId="29" borderId="0" xfId="111" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="79" fillId="29" borderId="0" xfId="111" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6497,8 +6497,8 @@
     </xf>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="204" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="204"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="204" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="66" fillId="25" borderId="16" xfId="205" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="204" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="66" fillId="25" borderId="16" xfId="205" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -6511,17 +6511,17 @@
     <xf numFmtId="14" fontId="1" fillId="29" borderId="0" xfId="204" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="204" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="204" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="0" fillId="29" borderId="0" xfId="206" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="184" fontId="0" fillId="29" borderId="0" xfId="206" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="82" fillId="31" borderId="7" xfId="204" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="183" fontId="82" fillId="31" borderId="7" xfId="204" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="82" fillId="31" borderId="7" xfId="204" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="82" fillId="31" borderId="7" xfId="204" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="92" fillId="29" borderId="0" xfId="207" applyFill="1"/>
     <xf numFmtId="43" fontId="92" fillId="29" borderId="0" xfId="124" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="92" fillId="29" borderId="0" xfId="207" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="207" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="92" fillId="29" borderId="0" xfId="207" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="92" fillId="29" borderId="0" xfId="207" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="207"/>
     <xf numFmtId="0" fontId="80" fillId="27" borderId="58" xfId="208" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6535,16 +6535,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="92" fillId="29" borderId="0" xfId="207" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="182" fontId="1" fillId="29" borderId="60" xfId="209" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="183" fontId="1" fillId="29" borderId="60" xfId="209" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="82" fillId="29" borderId="0" xfId="207" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="29" borderId="0" xfId="207" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="29" borderId="0" xfId="207" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="182" fontId="81" fillId="34" borderId="20" xfId="209" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="82" fillId="34" borderId="20" xfId="209" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="183" fontId="81" fillId="34" borderId="20" xfId="209" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="183" fontId="82" fillId="34" borderId="20" xfId="209" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="87" fillId="29" borderId="0" xfId="208" applyFont="1" applyFill="1"/>
-    <xf numFmtId="182" fontId="92" fillId="29" borderId="0" xfId="207" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="183" fontId="92" fillId="29" borderId="0" xfId="207" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="92" fillId="29" borderId="0" xfId="207" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="207" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="207" applyFill="1"/>
@@ -6552,7 +6552,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="207" applyFont="1" applyFill="1"/>
-    <xf numFmtId="182" fontId="92" fillId="0" borderId="0" xfId="207" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="92" fillId="0" borderId="0" xfId="207" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="207" applyFont="1"/>
     <xf numFmtId="0" fontId="126" fillId="29" borderId="0" xfId="211" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="212"/>
@@ -6571,27 +6571,27 @@
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" xfId="206" applyFont="1"/>
     <xf numFmtId="0" fontId="130" fillId="36" borderId="5" xfId="212" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="212" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="89" fillId="26" borderId="19" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="26" borderId="19" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="26" borderId="7" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="26" borderId="7" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="26" borderId="20" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="26" borderId="20" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="26" borderId="5" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="26" borderId="5" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="26" borderId="24" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="26" borderId="24" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -6607,10 +6607,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="40" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="40" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -6623,11 +6623,11 @@
     <xf numFmtId="4" fontId="89" fillId="0" borderId="40" xfId="114" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="5" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="5" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="5" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="5" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="4" fontId="89" fillId="0" borderId="5" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6636,24 +6636,24 @@
     <xf numFmtId="4" fontId="89" fillId="0" borderId="41" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="131" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="131" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="131" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="131" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="4" fontId="131" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="131" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="131" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="4" fontId="131" fillId="0" borderId="40" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="5" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="5" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -6664,7 +6664,7 @@
     <xf numFmtId="4" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -6675,35 +6675,35 @@
     <xf numFmtId="4" fontId="89" fillId="0" borderId="5" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="5" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="5" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="90" fillId="0" borderId="5" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="90" fillId="0" borderId="5" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="4" fontId="89" fillId="0" borderId="42" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="40" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="40" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="0" borderId="40" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="89" fillId="0" borderId="40" xfId="137" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="52" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6732,7 +6732,7 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="53" fillId="0" borderId="18" xfId="90" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="53" fillId="0" borderId="18" xfId="90" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="66" applyFont="1" applyAlignment="1">
@@ -6747,11 +6747,11 @@
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="66" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="66" fillId="25" borderId="25" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="66" fillId="25" borderId="25" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="66" fillId="25" borderId="16" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="66" fillId="25" borderId="16" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -6761,7 +6761,7 @@
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="66" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="51" fillId="24" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -6771,10 +6771,10 @@
     <xf numFmtId="0" fontId="80" fillId="27" borderId="54" xfId="208" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="81" fillId="34" borderId="7" xfId="210" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="81" fillId="34" borderId="7" xfId="210" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="81" fillId="34" borderId="26" xfId="210" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="81" fillId="34" borderId="26" xfId="210" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="80" fillId="27" borderId="49" xfId="208" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6804,11 +6804,23 @@
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="137" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="129" fillId="29" borderId="47" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="129" fillId="29" borderId="47" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="129" fillId="29" borderId="0" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="129" fillId="29" borderId="0" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="129" fillId="36" borderId="61" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="129" fillId="36" borderId="5" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="29" borderId="18" xfId="212" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="29" borderId="0" xfId="212" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="127" fillId="35" borderId="20" xfId="212" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6816,41 +6828,29 @@
     <xf numFmtId="0" fontId="127" fillId="35" borderId="7" xfId="212" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="129" fillId="36" borderId="47" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="129" fillId="36" borderId="47" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="129" fillId="36" borderId="0" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="129" fillId="36" borderId="0" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="129" fillId="29" borderId="61" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="129" fillId="29" borderId="61" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="129" fillId="29" borderId="5" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="129" fillId="29" borderId="5" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="130" fillId="36" borderId="47" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="130" fillId="36" borderId="47" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="130" fillId="36" borderId="0" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="130" fillId="36" borderId="0" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="129" fillId="36" borderId="61" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="129" fillId="36" borderId="5" xfId="213" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="29" borderId="18" xfId="212" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="29" borderId="0" xfId="212" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="89" fillId="26" borderId="7" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="26" borderId="7" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="89" fillId="26" borderId="26" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="89" fillId="26" borderId="26" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -7549,22 +7549,22 @@
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="93.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="1" customWidth="1"/>
-    <col min="4" max="6" width="12.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="19.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="93.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="12.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="19.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" style="135" customWidth="1"/>
-    <col min="15" max="15" width="9.1640625" style="1"/>
-    <col min="16" max="16" width="14.33203125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1640625" style="1"/>
+    <col min="12" max="12" width="24.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="135" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="14.28515625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" customFormat="1" ht="15" customHeight="1">
@@ -8116,7 +8116,7 @@
       <c r="M24" s="135"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" ht="16">
+    <row r="25" spans="1:14" ht="15.75">
       <c r="A25" s="227" t="s">
         <v>435</v>
       </c>
@@ -8147,7 +8147,7 @@
       <c r="M25" s="135"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" ht="16">
+    <row r="26" spans="1:14" ht="15.75">
       <c r="A26" s="226"/>
       <c r="B26" s="226"/>
       <c r="C26" s="226"/>
@@ -8160,7 +8160,7 @@
       <c r="M26" s="135"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" ht="16">
+    <row r="27" spans="1:14" ht="15.75">
       <c r="A27" s="227" t="s">
         <v>319</v>
       </c>
@@ -8191,7 +8191,7 @@
       <c r="M27" s="135"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:14" s="305" customFormat="1" ht="16" hidden="1">
+    <row r="28" spans="1:14" s="305" customFormat="1" ht="15.75" hidden="1">
       <c r="A28" s="303"/>
       <c r="B28" s="304"/>
       <c r="C28" s="304"/>
@@ -8205,7 +8205,7 @@
       </c>
       <c r="M28" s="306"/>
     </row>
-    <row r="29" spans="1:14" ht="16" hidden="1">
+    <row r="29" spans="1:14" ht="15.75" hidden="1">
       <c r="A29" s="227" t="s">
         <v>326</v>
       </c>
@@ -8236,7 +8236,7 @@
       <c r="M29" s="135"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:14" ht="16" hidden="1">
+    <row r="30" spans="1:14" ht="15.75" hidden="1">
       <c r="A30" s="226"/>
       <c r="B30" s="226"/>
       <c r="C30" s="226"/>
@@ -8251,7 +8251,7 @@
       <c r="M30" s="135"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:14" ht="16" hidden="1">
+    <row r="31" spans="1:14" ht="15.75" hidden="1">
       <c r="A31" s="227" t="s">
         <v>327</v>
       </c>
@@ -8282,7 +8282,7 @@
       <c r="M31" s="135"/>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:14" ht="16" hidden="1">
+    <row r="32" spans="1:14" ht="15.75" hidden="1">
       <c r="A32" s="226"/>
       <c r="B32" s="226"/>
       <c r="C32" s="226"/>
@@ -8298,7 +8298,7 @@
       <c r="M32" s="135"/>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="1:14" ht="16" hidden="1">
+    <row r="33" spans="1:14" ht="15.75" hidden="1">
       <c r="A33" s="227" t="s">
         <v>341</v>
       </c>
@@ -8329,7 +8329,7 @@
       <c r="M33" s="135"/>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:14" ht="16" hidden="1">
+    <row r="34" spans="1:14" ht="15.75" hidden="1">
       <c r="A34" s="303"/>
       <c r="B34" s="304"/>
       <c r="C34" s="304"/>
@@ -8344,7 +8344,7 @@
       <c r="M34" s="135"/>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="1:14" ht="16" hidden="1">
+    <row r="35" spans="1:14" ht="15.75" hidden="1">
       <c r="A35" s="227" t="s">
         <v>345</v>
       </c>
@@ -8369,7 +8369,7 @@
       <c r="M35" s="135"/>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:14" s="305" customFormat="1" ht="16" hidden="1">
+    <row r="36" spans="1:14" s="305" customFormat="1" ht="15.75" hidden="1">
       <c r="A36" s="303"/>
       <c r="B36" s="304"/>
       <c r="C36" s="304"/>
@@ -8383,7 +8383,7 @@
       </c>
       <c r="M36" s="306"/>
     </row>
-    <row r="37" spans="1:14" ht="16" hidden="1">
+    <row r="37" spans="1:14" ht="15.75" hidden="1">
       <c r="A37" s="227" t="s">
         <v>342</v>
       </c>
@@ -8410,7 +8410,7 @@
       <c r="M37" s="135"/>
       <c r="N37" s="1"/>
     </row>
-    <row r="38" spans="1:14" ht="16">
+    <row r="38" spans="1:14" ht="15.75">
       <c r="A38" s="303"/>
       <c r="B38" s="304"/>
       <c r="C38" s="304"/>
@@ -8475,16 +8475,16 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="48" customWidth="1"/>
-    <col min="2" max="2" width="84.83203125" style="48" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.33203125" style="49" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="48"/>
+    <col min="1" max="1" width="2.42578125" style="48" customWidth="1"/>
+    <col min="2" max="2" width="84.85546875" style="48" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.28515625" style="49" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="48"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4" ht="16">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="511" t="s">
         <v>95</v>
       </c>
@@ -8492,7 +8492,7 @@
       <c r="C4" s="511"/>
       <c r="D4" s="50"/>
     </row>
-    <row r="5" spans="1:4" ht="16">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="512" t="s">
         <v>421</v>
       </c>
@@ -8506,7 +8506,7 @@
       <c r="C6" s="74"/>
       <c r="D6" s="52"/>
     </row>
-    <row r="7" spans="1:4" ht="17" thickBot="1">
+    <row r="7" spans="1:4" ht="16.5" thickBot="1">
       <c r="A7" s="73"/>
       <c r="B7" s="73"/>
       <c r="C7" s="75" t="s">
@@ -8548,7 +8548,7 @@
       <c r="C11" s="401"/>
       <c r="D11" s="52"/>
     </row>
-    <row r="12" spans="1:4" ht="16">
+    <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="76" t="s">
         <v>91</v>
       </c>
@@ -8566,7 +8566,7 @@
       <c r="C13" s="401"/>
       <c r="D13" s="52"/>
     </row>
-    <row r="14" spans="1:4" ht="16">
+    <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="76" t="s">
         <v>100</v>
       </c>
@@ -8584,7 +8584,7 @@
       <c r="C15" s="401"/>
       <c r="D15" s="52"/>
     </row>
-    <row r="16" spans="1:4" ht="19">
+    <row r="16" spans="1:4" ht="18">
       <c r="A16" s="76" t="s">
         <v>92</v>
       </c>
@@ -8620,7 +8620,7 @@
       <c r="C19" s="402"/>
       <c r="D19" s="52"/>
     </row>
-    <row r="20" spans="1:6" ht="17">
+    <row r="20" spans="1:6" ht="15.75">
       <c r="A20" s="76" t="s">
         <v>416</v>
       </c>
@@ -8638,7 +8638,7 @@
       <c r="C21" s="401"/>
       <c r="D21" s="52"/>
     </row>
-    <row r="22" spans="1:6" s="61" customFormat="1" ht="16">
+    <row r="22" spans="1:6" s="61" customFormat="1" ht="15.75">
       <c r="A22" s="403" t="s">
         <v>260</v>
       </c>
@@ -8675,7 +8675,7 @@
       <c r="B25" s="515"/>
       <c r="C25" s="515"/>
     </row>
-    <row r="26" spans="1:6" ht="14">
+    <row r="26" spans="1:6">
       <c r="A26" s="510"/>
       <c r="B26" s="510"/>
       <c r="C26" s="510"/>
@@ -8731,15 +8731,15 @@
       <selection activeCell="A31" sqref="A31:XFD44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -8763,7 +8763,7 @@
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>
     </row>
-    <row r="4" spans="1:7" ht="16">
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" s="516" t="s">
         <v>154</v>
       </c>
@@ -8773,14 +8773,14 @@
       <c r="E4" s="516"/>
       <c r="F4" s="127"/>
     </row>
-    <row r="5" spans="1:7" ht="16">
+    <row r="5" spans="1:7" ht="15.75">
       <c r="A5" s="65"/>
       <c r="B5" s="65"/>
       <c r="C5" s="65"/>
       <c r="D5" s="65"/>
       <c r="E5" s="36"/>
     </row>
-    <row r="6" spans="1:7" ht="17" thickBot="1">
+    <row r="6" spans="1:7" ht="16.5" thickBot="1">
       <c r="A6" s="65"/>
       <c r="B6" s="65"/>
       <c r="C6" s="65"/>
@@ -8804,7 +8804,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" thickTop="1">
+    <row r="8" spans="1:7" ht="16.5" thickTop="1">
       <c r="A8" s="65"/>
       <c r="B8" s="65"/>
       <c r="C8" s="65"/>
@@ -8827,14 +8827,14 @@
       </c>
       <c r="F9" s="114"/>
     </row>
-    <row r="10" spans="1:7" ht="16">
+    <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="70"/>
       <c r="B10" s="70"/>
       <c r="C10" s="70"/>
       <c r="D10" s="70"/>
       <c r="E10" s="260"/>
     </row>
-    <row r="11" spans="1:7" ht="16">
+    <row r="11" spans="1:7" ht="15.75">
       <c r="A11" s="70" t="s">
         <v>146</v>
       </c>
@@ -8867,7 +8867,7 @@
       </c>
       <c r="F12" s="116"/>
     </row>
-    <row r="13" spans="1:7" ht="16">
+    <row r="13" spans="1:7" ht="15.75">
       <c r="A13" s="70"/>
       <c r="B13" s="71" t="s">
         <v>105</v>
@@ -8883,7 +8883,7 @@
       </c>
       <c r="F13" s="116"/>
     </row>
-    <row r="14" spans="1:7" ht="16">
+    <row r="14" spans="1:7" ht="15.75">
       <c r="A14" s="70"/>
       <c r="B14" s="71" t="s">
         <v>106</v>
@@ -8898,7 +8898,7 @@
         <v>151814.72577318267</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16">
+    <row r="15" spans="1:7" ht="15.75">
       <c r="A15" s="70"/>
       <c r="B15" s="71" t="s">
         <v>107</v>
@@ -8913,7 +8913,7 @@
         <v>573117.11689201917</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16">
+    <row r="16" spans="1:7" ht="15.75">
       <c r="A16" s="70"/>
       <c r="B16" s="71" t="s">
         <v>108</v>
@@ -8928,7 +8928,7 @@
         <v>1332830.5044000444</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16">
+    <row r="17" spans="1:6" ht="15.75">
       <c r="A17" s="70"/>
       <c r="B17" s="71" t="s">
         <v>109</v>
@@ -8943,7 +8943,7 @@
         <v>50538944.143737115</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16">
+    <row r="18" spans="1:6" ht="15.75">
       <c r="A18" s="70"/>
       <c r="B18" s="71" t="s">
         <v>110</v>
@@ -8958,7 +8958,7 @@
         <v>177710.73392000594</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16">
+    <row r="19" spans="1:6" ht="15.75">
       <c r="A19" s="70"/>
       <c r="B19" s="71" t="s">
         <v>111</v>
@@ -8973,7 +8973,7 @@
         <v>84797209.067889184</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16">
+    <row r="20" spans="1:6" ht="15.75">
       <c r="A20" s="70"/>
       <c r="B20" s="71" t="s">
         <v>112</v>
@@ -8988,7 +8988,7 @@
         <v>20753994.265638713</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16">
+    <row r="21" spans="1:6" ht="15.75">
       <c r="A21" s="70"/>
       <c r="B21" s="71" t="s">
         <v>113</v>
@@ -9003,7 +9003,7 @@
         <v>133283.05044000444</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16">
+    <row r="22" spans="1:6" ht="15.75">
       <c r="A22" s="70"/>
       <c r="B22" s="71" t="s">
         <v>114</v>
@@ -9018,7 +9018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16">
+    <row r="23" spans="1:6" ht="15.75">
       <c r="A23" s="70"/>
       <c r="B23" s="70" t="s">
         <v>115</v>
@@ -9034,7 +9034,7 @@
       </c>
       <c r="F23" s="116"/>
     </row>
-    <row r="24" spans="1:6" ht="16">
+    <row r="24" spans="1:6" ht="15.75">
       <c r="A24" s="70"/>
       <c r="B24" s="71" t="s">
         <v>116</v>
@@ -9050,7 +9050,7 @@
       </c>
       <c r="F24" s="116"/>
     </row>
-    <row r="25" spans="1:6" ht="16">
+    <row r="25" spans="1:6" ht="15.75">
       <c r="A25" s="70"/>
       <c r="B25" s="71" t="s">
         <v>117</v>
@@ -9072,7 +9072,7 @@
       <c r="D26" s="70"/>
       <c r="E26" s="260"/>
     </row>
-    <row r="27" spans="1:6" ht="16">
+    <row r="27" spans="1:6" ht="15.75">
       <c r="A27" s="517" t="s">
         <v>118</v>
       </c>
@@ -9131,30 +9131,30 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20" style="270" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="270" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="270" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="270" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="270" customWidth="1"/>
-    <col min="6" max="12" width="17.83203125" style="244" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="270" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="270" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="270" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="270" customWidth="1"/>
+    <col min="6" max="12" width="17.85546875" style="244" customWidth="1"/>
     <col min="13" max="13" width="44" style="270" customWidth="1"/>
     <col min="14" max="14" width="26" style="270" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5" style="270" customWidth="1"/>
-    <col min="16" max="16" width="16.5" style="270" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1640625" style="270" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="270"/>
+    <col min="15" max="15" width="17.42578125" style="270" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" style="270" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="270" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="270"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="16" thickBot="1">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1">
       <c r="C2" s="46"/>
       <c r="E2" s="46">
         <v>1</v>
       </c>
       <c r="G2" s="398"/>
     </row>
-    <row r="3" spans="1:7" ht="66" thickTop="1" thickBot="1">
+    <row r="3" spans="1:7" ht="76.5" thickTop="1" thickBot="1">
       <c r="A3" s="128" t="s">
         <v>320</v>
       </c>
@@ -9171,7 +9171,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14" thickTop="1"/>
+    <row r="4" spans="1:7" ht="13.5" thickTop="1"/>
     <row r="5" spans="1:7" ht="15">
       <c r="A5" s="287" t="s">
         <v>210</v>
@@ -9213,7 +9213,7 @@
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
     </row>
-    <row r="8" spans="1:7" ht="14">
+    <row r="8" spans="1:7">
       <c r="A8" s="109" t="s">
         <v>334</v>
       </c>
@@ -9242,17 +9242,17 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="424"/>
-    <col min="2" max="2" width="38.6640625" style="429" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="429" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="429" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="429" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="424"/>
+    <col min="2" max="2" width="38.7109375" style="429" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="429" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="429" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="429" customWidth="1"/>
     <col min="6" max="11" width="19" style="429" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.5" style="429" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="429" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1640625" style="429"/>
+    <col min="12" max="12" width="27.42578125" style="429" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="429" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="429"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="424" customFormat="1">
@@ -9265,13 +9265,13 @@
       <c r="L2" s="427"/>
     </row>
     <row r="3" spans="2:13" s="424" customFormat="1"/>
-    <row r="4" spans="2:13" s="424" customFormat="1" ht="16" thickBot="1">
+    <row r="4" spans="2:13" s="424" customFormat="1" ht="15.75" thickBot="1">
       <c r="I4" s="428"/>
       <c r="K4" s="428">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="16" thickTop="1">
+    <row r="5" spans="2:13" ht="15.75" thickTop="1">
       <c r="B5" s="522" t="s">
         <v>465</v>
       </c>
@@ -9297,7 +9297,7 @@
       </c>
       <c r="K5" s="519"/>
     </row>
-    <row r="6" spans="2:13" ht="16" thickBot="1">
+    <row r="6" spans="2:13" ht="15.75" thickBot="1">
       <c r="B6" s="523"/>
       <c r="C6" s="525"/>
       <c r="D6" s="525"/>
@@ -9322,7 +9322,7 @@
       </c>
       <c r="L6" s="432"/>
     </row>
-    <row r="7" spans="2:13" s="424" customFormat="1" ht="16" thickTop="1">
+    <row r="7" spans="2:13" s="424" customFormat="1" ht="15.75" thickTop="1">
       <c r="B7" s="433" t="s">
         <v>472</v>
       </c>
@@ -9784,89 +9784,89 @@
       <selection pane="bottomRight" activeCell="AZ36" sqref="AZ36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="98.1640625" style="321" customWidth="1"/>
-    <col min="2" max="3" width="11.83203125" style="321" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="14.6640625" style="321" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="321" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="98.140625" style="321" customWidth="1"/>
+    <col min="2" max="3" width="11.85546875" style="321" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="14.7109375" style="321" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="321" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="321" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5" style="321" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" style="321" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="2.5" style="321" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" style="321" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="1.33203125" style="321" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" style="321" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="2.33203125" style="321" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" style="321" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="321" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="2.42578125" style="321" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" style="321" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="1.28515625" style="321" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" style="321" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="2.28515625" style="321" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="321" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="0.5" style="321" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" style="321" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="1.6640625" style="321" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="0.33203125" style="321" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="14.1640625" style="321" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="1.83203125" style="321" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="0.42578125" style="321" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="321" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="1.7109375" style="321" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="0.28515625" style="321" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" style="321" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="1.85546875" style="321" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="1.83203125" style="321" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="1.85546875" style="321" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="1.83203125" style="321" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="1.85546875" style="321" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="1.83203125" style="321" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="1.85546875" style="321" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="0.5" style="321" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="0.42578125" style="321" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="0.5" style="321" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="0.42578125" style="321" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="0.5" style="321" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="0.5" style="322" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="0.42578125" style="321" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="0.42578125" style="322" hidden="1" customWidth="1"/>
     <col min="36" max="36" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="1.5" style="321" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="11.83203125" style="321" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="0.6640625" style="322" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="1.42578125" style="321" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="11.85546875" style="321" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="0.7109375" style="322" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="0.5" style="322" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="0.42578125" style="322" hidden="1" customWidth="1"/>
     <col min="42" max="42" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="0.5" style="322" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="0.42578125" style="322" hidden="1" customWidth="1"/>
     <col min="44" max="44" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="0.5" style="322" hidden="1" customWidth="1"/>
+    <col min="45" max="45" width="0.42578125" style="322" hidden="1" customWidth="1"/>
     <col min="46" max="46" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="0.5" style="322" customWidth="1"/>
+    <col min="47" max="47" width="0.42578125" style="322" customWidth="1"/>
     <col min="48" max="48" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="0.5" style="322" customWidth="1"/>
+    <col min="49" max="49" width="0.42578125" style="322" customWidth="1"/>
     <col min="50" max="50" width="14" style="321" customWidth="1"/>
-    <col min="51" max="51" width="0.5" style="322" customWidth="1"/>
+    <col min="51" max="51" width="0.42578125" style="322" customWidth="1"/>
     <col min="52" max="52" width="14" style="321" customWidth="1"/>
-    <col min="53" max="53" width="0.5" style="322" customWidth="1"/>
+    <col min="53" max="53" width="0.42578125" style="322" customWidth="1"/>
     <col min="54" max="54" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="0.5" style="322" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="0.42578125" style="322" hidden="1" customWidth="1"/>
     <col min="56" max="56" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="57" max="57" width="0.5" style="322" hidden="1" customWidth="1"/>
+    <col min="57" max="57" width="0.42578125" style="322" hidden="1" customWidth="1"/>
     <col min="58" max="58" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="0.5" style="322" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="0.42578125" style="322" hidden="1" customWidth="1"/>
     <col min="60" max="60" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="0.5" style="322" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="0.42578125" style="322" hidden="1" customWidth="1"/>
     <col min="62" max="62" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="1.1640625" style="322" hidden="1" customWidth="1"/>
+    <col min="63" max="63" width="1.140625" style="322" hidden="1" customWidth="1"/>
     <col min="64" max="65" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="0.5" style="322" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="0.42578125" style="322" hidden="1" customWidth="1"/>
     <col min="67" max="67" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="0.5" style="322" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="0.42578125" style="322" hidden="1" customWidth="1"/>
     <col min="69" max="69" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="1.1640625" style="322" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="1.140625" style="322" hidden="1" customWidth="1"/>
     <col min="71" max="71" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="72" max="72" width="1.1640625" style="322" hidden="1" customWidth="1"/>
+    <col min="72" max="72" width="1.140625" style="322" hidden="1" customWidth="1"/>
     <col min="73" max="73" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="74" max="74" width="1.1640625" style="322" hidden="1" customWidth="1"/>
+    <col min="74" max="74" width="1.140625" style="322" hidden="1" customWidth="1"/>
     <col min="75" max="75" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="76" max="76" width="1.1640625" style="322" hidden="1" customWidth="1"/>
+    <col min="76" max="76" width="1.140625" style="322" hidden="1" customWidth="1"/>
     <col min="77" max="77" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="78" max="78" width="1.1640625" style="322" hidden="1" customWidth="1"/>
+    <col min="78" max="78" width="1.140625" style="322" hidden="1" customWidth="1"/>
     <col min="79" max="79" width="14" style="321" hidden="1" customWidth="1"/>
-    <col min="80" max="80" width="20.83203125" style="322" hidden="1" customWidth="1"/>
+    <col min="80" max="80" width="20.85546875" style="322" hidden="1" customWidth="1"/>
     <col min="81" max="81" width="0" style="322" hidden="1" customWidth="1"/>
-    <col min="82" max="16384" width="9.1640625" style="322"/>
+    <col min="82" max="16384" width="9.140625" style="322"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" ht="19">
+    <row r="1" spans="1:79" ht="18.75">
       <c r="A1" s="529" t="s">
         <v>354</v>
       </c>
@@ -9892,7 +9892,7 @@
       <c r="U1" s="529"/>
       <c r="V1" s="320"/>
     </row>
-    <row r="4" spans="1:79" ht="15" thickBot="1">
+    <row r="4" spans="1:79" ht="13.5" thickBot="1">
       <c r="M4" s="323"/>
       <c r="N4" s="323"/>
       <c r="O4" s="323"/>
@@ -10131,7 +10131,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="6" spans="1:79" ht="16" thickTop="1">
+    <row r="6" spans="1:79" ht="15.75" thickTop="1">
       <c r="A6" s="330"/>
       <c r="B6" s="331"/>
       <c r="C6" s="330"/>
@@ -10139,7 +10139,7 @@
       <c r="E6" s="330"/>
       <c r="AJ6" s="332"/>
     </row>
-    <row r="7" spans="1:79" ht="17">
+    <row r="7" spans="1:79" ht="15.75">
       <c r="A7" s="333" t="s">
         <v>388</v>
       </c>
@@ -10308,7 +10308,7 @@
         <v>2232394.4797136174</v>
       </c>
     </row>
-    <row r="8" spans="1:79" ht="17">
+    <row r="8" spans="1:79" ht="15.75">
       <c r="A8" s="333" t="s">
         <v>429</v>
       </c>
@@ -11820,7 +11820,7 @@
       <c r="BZ17" s="347"/>
       <c r="CA17" s="341"/>
     </row>
-    <row r="18" spans="1:80" ht="16">
+    <row r="18" spans="1:80" ht="15.75">
       <c r="A18" s="349" t="s">
         <v>397</v>
       </c>
@@ -14802,7 +14802,7 @@
         <v>-1390.5867369307957</v>
       </c>
     </row>
-    <row r="36" spans="1:81" ht="16">
+    <row r="36" spans="1:81" ht="15.75">
       <c r="A36" s="349" t="s">
         <v>430</v>
       </c>
@@ -15052,7 +15052,7 @@
       <c r="BZ37" s="369"/>
       <c r="CA37" s="370"/>
     </row>
-    <row r="38" spans="1:81" ht="34" hidden="1">
+    <row r="38" spans="1:81" ht="31.5" hidden="1">
       <c r="A38" s="333" t="s">
         <v>408</v>
       </c>
@@ -15218,7 +15218,7 @@
       <c r="BZ39" s="369"/>
       <c r="CA39" s="370"/>
     </row>
-    <row r="40" spans="1:81" ht="34">
+    <row r="40" spans="1:81" ht="31.5">
       <c r="A40" s="333" t="s">
         <v>436</v>
       </c>
@@ -15470,7 +15470,7 @@
       <c r="CB41" s="363"/>
       <c r="CC41" s="372"/>
     </row>
-    <row r="42" spans="1:81" ht="17">
+    <row r="42" spans="1:81" ht="15.75">
       <c r="A42" s="333" t="s">
         <v>431</v>
       </c>
@@ -16058,8 +16058,8 @@
       <c r="K48" s="530"/>
       <c r="L48" s="530"/>
     </row>
-    <row r="50" spans="1:79" ht="15" thickBot="1"/>
-    <row r="51" spans="1:79" ht="15" thickBot="1">
+    <row r="50" spans="1:79" ht="13.5" thickBot="1"/>
+    <row r="51" spans="1:79" ht="13.5" thickBot="1">
       <c r="A51" s="388" t="s">
         <v>412</v>
       </c>
@@ -16374,16 +16374,16 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" style="452" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" style="452" customWidth="1"/>
-    <col min="4" max="8" width="9.1640625" style="452"/>
-    <col min="9" max="9" width="10.83203125" style="452" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1640625" style="452"/>
+    <col min="1" max="1" width="70.7109375" style="452" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" style="452" customWidth="1"/>
+    <col min="4" max="8" width="9.140625" style="452"/>
+    <col min="9" max="9" width="10.85546875" style="452" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="452"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19">
+    <row r="1" spans="1:9" ht="18.75">
       <c r="A1" s="451" t="s">
         <v>485</v>
       </c>
@@ -16397,19 +16397,19 @@
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1">
       <c r="A3" s="455"/>
-      <c r="B3" s="533" t="s">
+      <c r="B3" s="537" t="s">
         <v>487</v>
       </c>
-      <c r="C3" s="534"/>
+      <c r="C3" s="538"/>
     </row>
     <row r="4" spans="1:9" ht="27.75" customHeight="1">
       <c r="A4" s="456" t="s">
         <v>488</v>
       </c>
-      <c r="B4" s="535">
+      <c r="B4" s="539">
         <v>1671.4742038213162</v>
       </c>
-      <c r="C4" s="536"/>
+      <c r="C4" s="540"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1">
       <c r="A5" s="457" t="s">
@@ -16424,19 +16424,19 @@
       <c r="A6" s="457" t="s">
         <v>490</v>
       </c>
-      <c r="B6" s="537">
+      <c r="B6" s="541">
         <v>123.22377078287514</v>
       </c>
-      <c r="C6" s="538"/>
+      <c r="C6" s="542"/>
     </row>
     <row r="7" spans="1:9" ht="27.75" customHeight="1">
       <c r="A7" s="458" t="s">
         <v>491</v>
       </c>
-      <c r="B7" s="539">
+      <c r="B7" s="543">
         <v>1686.5791131000001</v>
       </c>
-      <c r="C7" s="540"/>
+      <c r="C7" s="544"/>
     </row>
     <row r="8" spans="1:9" ht="27.75" customHeight="1">
       <c r="A8" s="457" t="s">
@@ -16470,40 +16470,40 @@
       <c r="A11" s="460" t="s">
         <v>495</v>
       </c>
-      <c r="B11" s="541">
+      <c r="B11" s="533">
         <v>15.104909278683863</v>
       </c>
-      <c r="C11" s="542"/>
+      <c r="C11" s="534"/>
     </row>
     <row r="12" spans="1:9" ht="42.75" customHeight="1">
-      <c r="A12" s="543" t="s">
+      <c r="A12" s="535" t="s">
         <v>496</v>
       </c>
-      <c r="B12" s="543"/>
-      <c r="C12" s="543"/>
+      <c r="B12" s="535"/>
+      <c r="C12" s="535"/>
       <c r="I12" s="461"/>
     </row>
     <row r="13" spans="1:9" ht="37.5" customHeight="1">
-      <c r="A13" s="544" t="s">
+      <c r="A13" s="536" t="s">
         <v>497</v>
       </c>
-      <c r="B13" s="544"/>
-      <c r="C13" s="544"/>
+      <c r="B13" s="536"/>
+      <c r="C13" s="536"/>
       <c r="I13" s="461"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16521,21 +16521,21 @@
       <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.5" style="148" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" style="148" customWidth="1"/>
-    <col min="3" max="3" width="81.6640625" style="148" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="148" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="148" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="148" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="148" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5" style="277" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="1.5" style="148" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="4.1640625" style="148" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="81.6640625" style="148" hidden="1" customWidth="1"/>
-    <col min="12" max="15" width="16.33203125" style="148" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="20.6640625" style="148"/>
+    <col min="1" max="1" width="1.42578125" style="148" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="148" customWidth="1"/>
+    <col min="3" max="3" width="81.7109375" style="148" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="148" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="148" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="148" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="148" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" style="277" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="1.42578125" style="148" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" style="148" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="81.7109375" style="148" hidden="1" customWidth="1"/>
+    <col min="12" max="15" width="16.28515625" style="148" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="20.7109375" style="148"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
@@ -18077,7 +18077,7 @@
         <v>8941.7155921202211</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="20" hidden="1">
+    <row r="44" spans="1:15" ht="19.5" hidden="1">
       <c r="A44" s="154"/>
       <c r="B44" s="166"/>
       <c r="C44" s="168" t="s">
@@ -19714,7 +19714,7 @@
       <c r="N90" s="157"/>
       <c r="O90" s="157"/>
     </row>
-    <row r="91" spans="1:15" s="181" customFormat="1" ht="15.5" customHeight="1">
+    <row r="91" spans="1:15" s="181" customFormat="1" ht="15.6" customHeight="1">
       <c r="A91" s="162" t="s">
         <v>195</v>
       </c>
@@ -20518,19 +20518,19 @@
       <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.33203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
-    <col min="5" max="9" width="17.5" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" style="1" customWidth="1"/>
-    <col min="11" max="12" width="7.33203125" style="1"/>
-    <col min="13" max="13" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.33203125" style="1"/>
-    <col min="16" max="16" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="7.33203125" style="1"/>
+    <col min="1" max="1" width="40.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="9" width="17.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="7.28515625" style="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.28515625" style="1"/>
+    <col min="16" max="16" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="7.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -20568,7 +20568,7 @@
       <c r="H5" s="273"/>
       <c r="I5" s="315"/>
     </row>
-    <row r="6" spans="1:17" ht="70" thickTop="1" thickBot="1">
+    <row r="6" spans="1:17" ht="64.5" thickTop="1" thickBot="1">
       <c r="A6" s="38" t="s">
         <v>22</v>
       </c>
@@ -21015,23 +21015,23 @@
   </sheetPr>
   <dimension ref="A4:Z67"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A29" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="60" style="12" customWidth="1"/>
-    <col min="2" max="3" width="19.5" style="12" customWidth="1"/>
-    <col min="4" max="8" width="19.5" style="12" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5" style="12" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="38.5" style="12" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" style="12"/>
-    <col min="13" max="13" width="29.1640625" style="12" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" style="12"/>
-    <col min="15" max="15" width="9.1640625" style="12" customWidth="1"/>
-    <col min="16" max="16384" width="9.1640625" style="12"/>
+    <col min="2" max="3" width="19.42578125" style="12" customWidth="1"/>
+    <col min="4" max="8" width="19.42578125" style="12" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="12" customWidth="1"/>
+    <col min="11" max="11" width="38.42578125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="12"/>
+    <col min="13" max="13" width="29.140625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="12"/>
+    <col min="15" max="15" width="9.140625" style="12" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:26" ht="18.75" customHeight="1" thickBot="1">
@@ -21095,7 +21095,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:26" ht="16">
+    <row r="7" spans="1:26" ht="15.75">
       <c r="A7" s="41" t="s">
         <v>2</v>
       </c>
@@ -21921,7 +21921,7 @@
       <c r="J33" s="17"/>
       <c r="P33" s="16"/>
     </row>
-    <row r="34" spans="1:16" ht="17">
+    <row r="34" spans="1:16" ht="15.75">
       <c r="A34" s="110" t="s">
         <v>152</v>
       </c>
@@ -22289,10 +22289,10 @@
     <row r="58" spans="1:9" ht="18.75" customHeight="1">
       <c r="A58" s="132"/>
     </row>
-    <row r="59" spans="1:9" ht="16">
+    <row r="59" spans="1:9" ht="15.75">
       <c r="A59" s="131"/>
     </row>
-    <row r="60" spans="1:9" ht="16">
+    <row r="60" spans="1:9" ht="15.75">
       <c r="A60" s="131"/>
     </row>
     <row r="61" spans="1:9" ht="18.75" customHeight="1">
@@ -22336,7 +22336,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
@@ -22356,18 +22356,18 @@
   <dimension ref="B2:K38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="0" style="12" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5" style="12" customWidth="1"/>
-    <col min="3" max="4" width="16.6640625" style="12" customWidth="1"/>
-    <col min="5" max="9" width="16.6640625" style="12" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" style="12"/>
+    <col min="2" max="2" width="63.42578125" style="12" customWidth="1"/>
+    <col min="3" max="4" width="16.7109375" style="12" customWidth="1"/>
+    <col min="5" max="9" width="16.7109375" style="12" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="30.75" customHeight="1">
@@ -22438,8 +22438,8 @@
         <v>499</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="15" customHeight="1" thickTop="1"/>
-    <row r="7" spans="2:11" ht="15" customHeight="1">
+    <row r="6" spans="2:11" ht="16.5" thickTop="1"/>
+    <row r="7" spans="2:11" ht="15.75">
       <c r="B7" s="137" t="s">
         <v>132</v>
       </c>
@@ -22471,7 +22471,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="15" customHeight="1">
+    <row r="8" spans="2:11" ht="15.75">
       <c r="B8" s="138" t="s">
         <v>119</v>
       </c>
@@ -22503,7 +22503,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="15" customHeight="1">
+    <row r="9" spans="2:11" ht="15.75">
       <c r="B9" s="139" t="s">
         <v>120</v>
       </c>
@@ -22535,7 +22535,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="15" customHeight="1">
+    <row r="10" spans="2:11" ht="15.75">
       <c r="B10" s="138" t="s">
         <v>121</v>
       </c>
@@ -22564,7 +22564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="15" hidden="1" customHeight="1">
+    <row r="11" spans="2:11" ht="15.75">
       <c r="B11" s="139" t="s">
         <v>165</v>
       </c>
@@ -22593,7 +22593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="15" hidden="1" customHeight="1">
+    <row r="12" spans="2:11" ht="15.75">
       <c r="B12" s="138" t="s">
         <v>158</v>
       </c>
@@ -22622,7 +22622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="15" customHeight="1">
+    <row r="13" spans="2:11" ht="15.75">
       <c r="B13" s="138" t="s">
         <v>157</v>
       </c>
@@ -22651,7 +22651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="15" customHeight="1">
+    <row r="14" spans="2:11" ht="15.75">
       <c r="B14" s="138" t="s">
         <v>122</v>
       </c>
@@ -22683,7 +22683,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="15" customHeight="1">
+    <row r="15" spans="2:11" ht="15.75">
       <c r="B15" s="138" t="s">
         <v>241</v>
       </c>
@@ -22712,7 +22712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="15" customHeight="1">
+    <row r="16" spans="2:11" ht="15.75">
       <c r="B16" s="138" t="s">
         <v>123</v>
       </c>
@@ -22744,7 +22744,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15" customHeight="1">
+    <row r="17" spans="2:11" ht="15.75">
       <c r="B17" s="139" t="s">
         <v>131</v>
       </c>
@@ -22776,7 +22776,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="16" hidden="1">
+    <row r="18" spans="2:11" ht="15.75">
       <c r="B18" s="138" t="s">
         <v>124</v>
       </c>
@@ -22805,7 +22805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="16">
+    <row r="19" spans="2:11" ht="15.75">
       <c r="B19" s="138" t="s">
         <v>125</v>
       </c>
@@ -22834,7 +22834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15" customHeight="1">
+    <row r="20" spans="2:11" ht="15.75">
       <c r="B20" s="139" t="s">
         <v>275</v>
       </c>
@@ -22866,7 +22866,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="15" customHeight="1">
+    <row r="21" spans="2:11" ht="15.75">
       <c r="B21" s="138" t="s">
         <v>242</v>
       </c>
@@ -22898,7 +22898,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="15" hidden="1" customHeight="1">
+    <row r="22" spans="2:11" ht="15.75">
       <c r="B22" s="138" t="s">
         <v>126</v>
       </c>
@@ -22927,7 +22927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="17.25" customHeight="1">
+    <row r="23" spans="2:11" ht="15.75">
       <c r="B23" s="187" t="s">
         <v>243</v>
       </c>
@@ -22959,7 +22959,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="15" customHeight="1">
+    <row r="24" spans="2:11" ht="15.75">
       <c r="B24" s="138" t="s">
         <v>311</v>
       </c>
@@ -22988,7 +22988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="15" customHeight="1">
+    <row r="25" spans="2:11" ht="15.75">
       <c r="B25" s="138" t="s">
         <v>127</v>
       </c>
@@ -23020,7 +23020,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="15" customHeight="1">
+    <row r="26" spans="2:11" ht="15.75">
       <c r="B26" s="138" t="s">
         <v>244</v>
       </c>
@@ -23052,7 +23052,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="15" customHeight="1">
+    <row r="27" spans="2:11" ht="15.75">
       <c r="B27" s="138" t="s">
         <v>128</v>
       </c>
@@ -23084,7 +23084,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="15" customHeight="1">
+    <row r="28" spans="2:11" ht="15.75">
       <c r="B28" s="137" t="s">
         <v>129</v>
       </c>
@@ -23116,7 +23116,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="15" customHeight="1">
+    <row r="29" spans="2:11" ht="15.75">
       <c r="B29" s="137" t="s">
         <v>130</v>
       </c>
@@ -23148,7 +23148,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="15" customHeight="1">
+    <row r="30" spans="2:11" ht="15.75">
       <c r="B30" s="137" t="s">
         <v>199</v>
       </c>
@@ -23180,7 +23180,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="15" hidden="1" customHeight="1">
+    <row r="31" spans="2:11" ht="15.75">
       <c r="B31" s="137" t="s">
         <v>203</v>
       </c>
@@ -23209,7 +23209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="15" customHeight="1">
+    <row r="32" spans="2:11" ht="15.75">
       <c r="B32" s="250" t="s">
         <v>288</v>
       </c>
@@ -23238,7 +23238,7 @@
         <v>445.7445000000298</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="15" customHeight="1">
+    <row r="33" spans="2:11" ht="409.5">
       <c r="B33" s="251" t="s">
         <v>204</v>
       </c>
@@ -23270,7 +23270,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="15" customHeight="1">
+    <row r="34" spans="2:11" ht="15.75">
       <c r="B34" s="253" t="s">
         <v>276</v>
       </c>
@@ -23372,17 +23372,17 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.5" style="410" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="410" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="410" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.33203125" style="410" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="410" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1640625" style="410"/>
+    <col min="1" max="1" width="33.42578125" style="410" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="410" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="410" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.28515625" style="410" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="410" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="410"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -23395,12 +23395,12 @@
       <c r="E1" s="505"/>
       <c r="F1" s="409"/>
     </row>
-    <row r="2" spans="1:7" ht="16" thickBot="1">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1">
       <c r="E2" s="411">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19" thickTop="1" thickBot="1">
+    <row r="3" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
       <c r="A3" s="412" t="s">
         <v>440</v>
       </c>
@@ -23683,26 +23683,26 @@
   </sheetPr>
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A39" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="308" customWidth="1"/>
     <col min="2" max="2" width="84" style="190" customWidth="1"/>
-    <col min="3" max="4" width="20.83203125" style="189" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="189" hidden="1" customWidth="1"/>
-    <col min="6" max="8" width="18.33203125" style="189" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="189" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="22.6640625" style="189" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" style="235" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" style="189"/>
-    <col min="13" max="13" width="19.33203125" style="189" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1640625" style="189"/>
+    <col min="3" max="4" width="20.85546875" style="189" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="189" hidden="1" customWidth="1"/>
+    <col min="6" max="8" width="18.28515625" style="189" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="189" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" style="189" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="235" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="189"/>
+    <col min="13" max="13" width="19.28515625" style="189" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="189"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16">
+    <row r="1" spans="1:14" ht="15.75">
       <c r="A1" s="205"/>
       <c r="B1" s="205"/>
     </row>
@@ -23774,7 +23774,7 @@
       <c r="J6" s="270"/>
       <c r="K6" s="237"/>
     </row>
-    <row r="7" spans="1:14" s="194" customFormat="1" ht="19">
+    <row r="7" spans="1:14" s="194" customFormat="1" ht="34.5">
       <c r="A7" s="310">
         <v>8585</v>
       </c>
@@ -23807,7 +23807,7 @@
       </c>
       <c r="K7" s="236"/>
     </row>
-    <row r="8" spans="1:14" s="194" customFormat="1" ht="19">
+    <row r="8" spans="1:14" s="194" customFormat="1" ht="18.75">
       <c r="A8" s="310">
         <v>4295</v>
       </c>
@@ -23840,7 +23840,7 @@
       </c>
       <c r="K8" s="236"/>
     </row>
-    <row r="9" spans="1:14" s="195" customFormat="1" ht="36" hidden="1">
+    <row r="9" spans="1:14" s="195" customFormat="1" ht="34.5" hidden="1">
       <c r="A9" s="310">
         <v>8442</v>
       </c>
@@ -23873,7 +23873,7 @@
       </c>
       <c r="K9" s="236"/>
     </row>
-    <row r="10" spans="1:14" s="195" customFormat="1" ht="19">
+    <row r="10" spans="1:14" s="195" customFormat="1" ht="18.75">
       <c r="A10" s="310" t="s">
         <v>226</v>
       </c>
@@ -23937,7 +23937,7 @@
       </c>
       <c r="K11" s="236"/>
     </row>
-    <row r="12" spans="1:14" s="195" customFormat="1" ht="19">
+    <row r="12" spans="1:14" s="195" customFormat="1" ht="34.5">
       <c r="A12" s="310" t="s">
         <v>212</v>
       </c>
@@ -23970,7 +23970,7 @@
       </c>
       <c r="K12" s="236"/>
     </row>
-    <row r="13" spans="1:14" s="195" customFormat="1" ht="36">
+    <row r="13" spans="1:14" s="195" customFormat="1" ht="34.5">
       <c r="A13" s="310">
         <v>2004</v>
       </c>
@@ -24003,7 +24003,7 @@
       </c>
       <c r="K13" s="236"/>
     </row>
-    <row r="14" spans="1:14" s="195" customFormat="1" ht="36">
+    <row r="14" spans="1:14" s="195" customFormat="1" ht="34.5">
       <c r="A14" s="310">
         <v>4705</v>
       </c>
@@ -24036,7 +24036,7 @@
       </c>
       <c r="K14" s="236"/>
     </row>
-    <row r="15" spans="1:14" s="195" customFormat="1" ht="36">
+    <row r="15" spans="1:14" s="195" customFormat="1" ht="34.5">
       <c r="A15" s="310" t="s">
         <v>225</v>
       </c>
@@ -24069,7 +24069,7 @@
       </c>
       <c r="K15" s="236"/>
     </row>
-    <row r="16" spans="1:14" s="195" customFormat="1" ht="19">
+    <row r="16" spans="1:14" s="195" customFormat="1" ht="18.75">
       <c r="A16" s="310" t="s">
         <v>213</v>
       </c>
@@ -24102,7 +24102,7 @@
       </c>
       <c r="K16" s="236"/>
     </row>
-    <row r="17" spans="1:11" s="195" customFormat="1" ht="36">
+    <row r="17" spans="1:11" s="195" customFormat="1" ht="34.5">
       <c r="A17" s="310" t="s">
         <v>224</v>
       </c>
@@ -24135,7 +24135,7 @@
       </c>
       <c r="K17" s="236"/>
     </row>
-    <row r="18" spans="1:11" s="195" customFormat="1" ht="36">
+    <row r="18" spans="1:11" s="195" customFormat="1" ht="34.5">
       <c r="A18" s="310" t="s">
         <v>222</v>
       </c>
@@ -24168,7 +24168,7 @@
       </c>
       <c r="K18" s="236"/>
     </row>
-    <row r="19" spans="1:11" s="195" customFormat="1" ht="19">
+    <row r="19" spans="1:11" s="195" customFormat="1" ht="18.75">
       <c r="A19" s="310" t="s">
         <v>214</v>
       </c>
@@ -24201,7 +24201,7 @@
       </c>
       <c r="K19" s="236"/>
     </row>
-    <row r="20" spans="1:11" s="195" customFormat="1" ht="19">
+    <row r="20" spans="1:11" s="195" customFormat="1" ht="18.75">
       <c r="A20" s="310" t="s">
         <v>218</v>
       </c>
@@ -24267,7 +24267,7 @@
       </c>
       <c r="K21" s="236"/>
     </row>
-    <row r="22" spans="1:11" s="195" customFormat="1" ht="36">
+    <row r="22" spans="1:11" s="195" customFormat="1" ht="34.5">
       <c r="A22" s="310">
         <v>4370</v>
       </c>
@@ -24300,7 +24300,7 @@
       </c>
       <c r="K22" s="236"/>
     </row>
-    <row r="23" spans="1:11" s="195" customFormat="1" ht="36" hidden="1">
+    <row r="23" spans="1:11" s="195" customFormat="1" ht="51.75" hidden="1">
       <c r="A23" s="310" t="s">
         <v>216</v>
       </c>
@@ -24333,7 +24333,7 @@
       </c>
       <c r="K23" s="236"/>
     </row>
-    <row r="24" spans="1:11" s="195" customFormat="1" ht="19">
+    <row r="24" spans="1:11" s="195" customFormat="1" ht="18.75">
       <c r="A24" s="310" t="s">
         <v>219</v>
       </c>
@@ -24366,7 +24366,7 @@
       </c>
       <c r="K24" s="236"/>
     </row>
-    <row r="25" spans="1:11" s="195" customFormat="1" ht="19">
+    <row r="25" spans="1:11" s="195" customFormat="1" ht="18.75">
       <c r="A25" s="310" t="s">
         <v>215</v>
       </c>
@@ -24399,7 +24399,7 @@
       </c>
       <c r="K25" s="236"/>
     </row>
-    <row r="26" spans="1:11" s="195" customFormat="1" ht="19">
+    <row r="26" spans="1:11" s="195" customFormat="1" ht="18.75">
       <c r="A26" s="310" t="s">
         <v>211</v>
       </c>
@@ -24432,7 +24432,7 @@
       </c>
       <c r="K26" s="236"/>
     </row>
-    <row r="27" spans="1:11" s="195" customFormat="1" ht="19" hidden="1">
+    <row r="27" spans="1:11" s="195" customFormat="1" ht="18.75" hidden="1">
       <c r="A27" s="310">
         <v>8446</v>
       </c>
@@ -24465,7 +24465,7 @@
       </c>
       <c r="K27" s="236"/>
     </row>
-    <row r="28" spans="1:11" s="195" customFormat="1" ht="36">
+    <row r="28" spans="1:11" s="195" customFormat="1" ht="34.5">
       <c r="A28" s="310">
         <v>4368</v>
       </c>
@@ -24498,7 +24498,7 @@
       </c>
       <c r="K28" s="236"/>
     </row>
-    <row r="29" spans="1:11" s="195" customFormat="1" ht="19">
+    <row r="29" spans="1:11" s="195" customFormat="1" ht="18.75">
       <c r="A29" s="310">
         <v>2865</v>
       </c>
@@ -24531,7 +24531,7 @@
       </c>
       <c r="K29" s="236"/>
     </row>
-    <row r="30" spans="1:11" s="195" customFormat="1" ht="36">
+    <row r="30" spans="1:11" s="195" customFormat="1" ht="34.5">
       <c r="A30" s="310" t="s">
         <v>221</v>
       </c>
@@ -24564,7 +24564,7 @@
       </c>
       <c r="K30" s="236"/>
     </row>
-    <row r="31" spans="1:11" s="195" customFormat="1" ht="19" hidden="1">
+    <row r="31" spans="1:11" s="195" customFormat="1" ht="34.5" hidden="1">
       <c r="A31" s="310" t="s">
         <v>227</v>
       </c>
@@ -24597,7 +24597,7 @@
       </c>
       <c r="K31" s="236"/>
     </row>
-    <row r="32" spans="1:11" s="195" customFormat="1" ht="19" hidden="1">
+    <row r="32" spans="1:11" s="195" customFormat="1" ht="18.75" hidden="1">
       <c r="A32" s="311" t="s">
         <v>220</v>
       </c>
@@ -24630,7 +24630,7 @@
       </c>
       <c r="K32" s="236"/>
     </row>
-    <row r="33" spans="1:11" s="195" customFormat="1" ht="36">
+    <row r="33" spans="1:11" s="195" customFormat="1" ht="34.5">
       <c r="A33" s="310" t="s">
         <v>223</v>
       </c>
@@ -24663,7 +24663,7 @@
       </c>
       <c r="K33" s="236"/>
     </row>
-    <row r="34" spans="1:11" s="195" customFormat="1" ht="19">
+    <row r="34" spans="1:11" s="195" customFormat="1" ht="18.75">
       <c r="A34" s="310">
         <v>2913</v>
       </c>
@@ -24696,7 +24696,7 @@
       </c>
       <c r="K34" s="236"/>
     </row>
-    <row r="35" spans="1:11" s="195" customFormat="1" ht="19">
+    <row r="35" spans="1:11" s="195" customFormat="1" ht="18.75">
       <c r="A35" s="310" t="s">
         <v>228</v>
       </c>
@@ -24729,7 +24729,7 @@
       </c>
       <c r="K35" s="236"/>
     </row>
-    <row r="36" spans="1:11" s="211" customFormat="1" ht="19">
+    <row r="36" spans="1:11" s="211" customFormat="1" ht="18.75">
       <c r="A36" s="310">
         <v>30907</v>
       </c>
@@ -24762,7 +24762,7 @@
       </c>
       <c r="K36" s="236"/>
     </row>
-    <row r="37" spans="1:11" s="211" customFormat="1" ht="36" hidden="1">
+    <row r="37" spans="1:11" s="211" customFormat="1" ht="34.5" hidden="1">
       <c r="A37" s="310" t="s">
         <v>297</v>
       </c>
@@ -24795,7 +24795,7 @@
       </c>
       <c r="K37" s="236"/>
     </row>
-    <row r="38" spans="1:11" s="211" customFormat="1" ht="19">
+    <row r="38" spans="1:11" s="211" customFormat="1" ht="18.75">
       <c r="A38" s="310" t="s">
         <v>299</v>
       </c>
@@ -24828,7 +24828,7 @@
       </c>
       <c r="K38" s="236"/>
     </row>
-    <row r="39" spans="1:11" s="211" customFormat="1" ht="19">
+    <row r="39" spans="1:11" s="211" customFormat="1" ht="18.75">
       <c r="A39" s="310">
         <v>30911</v>
       </c>
@@ -24861,7 +24861,7 @@
       </c>
       <c r="K39" s="236"/>
     </row>
-    <row r="40" spans="1:11" s="211" customFormat="1" ht="19">
+    <row r="40" spans="1:11" s="211" customFormat="1" ht="18.75">
       <c r="A40" s="310" t="s">
         <v>331</v>
       </c>
@@ -24894,7 +24894,7 @@
       </c>
       <c r="K40" s="236"/>
     </row>
-    <row r="41" spans="1:11" s="211" customFormat="1" ht="36">
+    <row r="41" spans="1:11" s="211" customFormat="1" ht="34.5">
       <c r="A41" s="310" t="s">
         <v>350</v>
       </c>
@@ -24927,7 +24927,7 @@
       </c>
       <c r="K41" s="236"/>
     </row>
-    <row r="42" spans="1:11" s="211" customFormat="1" ht="36">
+    <row r="42" spans="1:11" s="211" customFormat="1" ht="34.5">
       <c r="A42" s="310" t="s">
         <v>351</v>
       </c>
@@ -25025,35 +25025,35 @@
       <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="2.1640625" customWidth="1"/>
-    <col min="9" max="9" width="2.1640625" style="93" customWidth="1"/>
-    <col min="10" max="10" width="2.1640625" style="36" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" customWidth="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="13.5" customWidth="1"/>
-    <col min="14" max="15" width="11.83203125" customWidth="1"/>
-    <col min="16" max="16" width="1.83203125" customWidth="1"/>
-    <col min="17" max="17" width="2.1640625" style="93" customWidth="1"/>
-    <col min="18" max="18" width="2.5" customWidth="1"/>
-    <col min="19" max="19" width="42.1640625" style="270" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.6640625" customWidth="1"/>
-    <col min="21" max="21" width="20.6640625" style="270" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" style="93" customWidth="1"/>
+    <col min="10" max="10" width="2.140625" style="36" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="15" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="1.85546875" customWidth="1"/>
+    <col min="17" max="17" width="2.140625" style="93" customWidth="1"/>
+    <col min="18" max="18" width="2.42578125" customWidth="1"/>
+    <col min="19" max="19" width="42.140625" style="270" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" style="270" customWidth="1"/>
     <col min="22" max="22" width="11" style="270" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.83203125" customWidth="1"/>
-    <col min="24" max="24" width="2.1640625" style="93" customWidth="1"/>
-    <col min="25" max="25" width="4.5" style="270" customWidth="1"/>
+    <col min="23" max="23" width="6.85546875" customWidth="1"/>
+    <col min="24" max="24" width="2.140625" style="93" customWidth="1"/>
+    <col min="25" max="25" width="4.42578125" style="270" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" thickBot="1">
+    <row r="1" spans="1:25" ht="13.5" thickBot="1">
       <c r="G1" s="92" t="s">
         <v>1</v>
       </c>
@@ -25068,7 +25068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="53" thickTop="1" thickBot="1">
+    <row r="2" spans="1:25" ht="48.75" thickTop="1" thickBot="1">
       <c r="A2" s="94" t="s">
         <v>134</v>
       </c>
@@ -25122,7 +25122,7 @@
       <c r="W2" s="270"/>
       <c r="Y2" s="312"/>
     </row>
-    <row r="3" spans="1:25" ht="16" thickTop="1">
+    <row r="3" spans="1:25" ht="15.75" thickTop="1">
       <c r="A3" s="213">
         <v>44562</v>
       </c>
@@ -25826,48 +25826,48 @@
       <c r="S20"/>
       <c r="V20"/>
     </row>
-    <row r="21" spans="8:22" ht="14">
+    <row r="21" spans="8:22">
       <c r="H21" s="91"/>
       <c r="O21" s="102"/>
       <c r="P21" s="91"/>
       <c r="S21"/>
       <c r="V21"/>
     </row>
-    <row r="22" spans="8:22" ht="14">
+    <row r="22" spans="8:22">
       <c r="H22" s="91"/>
       <c r="O22" s="102"/>
       <c r="P22" s="91"/>
       <c r="S22"/>
       <c r="V22"/>
     </row>
-    <row r="23" spans="8:22" ht="14">
+    <row r="23" spans="8:22">
       <c r="H23" s="91"/>
       <c r="O23" s="102"/>
       <c r="P23" s="91"/>
       <c r="S23"/>
       <c r="V23"/>
     </row>
-    <row r="24" spans="8:22" ht="14">
+    <row r="24" spans="8:22">
       <c r="O24" s="103"/>
       <c r="S24"/>
       <c r="V24"/>
     </row>
-    <row r="25" spans="8:22" ht="14">
+    <row r="25" spans="8:22">
       <c r="O25" s="104"/>
       <c r="S25"/>
       <c r="V25"/>
     </row>
-    <row r="26" spans="8:22" ht="14">
+    <row r="26" spans="8:22">
       <c r="O26" s="105"/>
       <c r="S26"/>
       <c r="V26"/>
     </row>
-    <row r="27" spans="8:22" ht="14">
+    <row r="27" spans="8:22">
       <c r="O27" s="106"/>
       <c r="S27"/>
       <c r="V27"/>
     </row>
-    <row r="28" spans="8:22" ht="14">
+    <row r="28" spans="8:22">
       <c r="O28" s="107"/>
       <c r="S28"/>
       <c r="V28"/>
@@ -25880,11 +25880,11 @@
       <c r="S30"/>
       <c r="V30"/>
     </row>
-    <row r="31" spans="8:22" ht="14" thickBot="1">
+    <row r="31" spans="8:22" ht="13.5" thickBot="1">
       <c r="S31"/>
       <c r="V31"/>
     </row>
-    <row r="32" spans="8:22" ht="14" thickBot="1">
+    <row r="32" spans="8:22" ht="13.5" thickBot="1">
       <c r="M32" s="241" t="s">
         <v>148</v>
       </c>
@@ -26036,18 +26036,18 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.5" style="12" customWidth="1"/>
-    <col min="4" max="8" width="15.5" style="12" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="38.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" style="12"/>
-    <col min="14" max="14" width="47.5" style="12" customWidth="1"/>
-    <col min="15" max="16384" width="9.1640625" style="12"/>
+    <col min="1" max="1" width="34.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" style="12" customWidth="1"/>
+    <col min="4" max="8" width="15.42578125" style="12" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="12" customWidth="1"/>
+    <col min="12" max="12" width="38.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="12"/>
+    <col min="14" max="14" width="47.42578125" style="12" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1">
@@ -26062,7 +26062,7 @@
       <c r="I1" s="270"/>
       <c r="J1"/>
     </row>
-    <row r="2" spans="1:16" ht="17" thickBot="1">
+    <row r="2" spans="1:16" ht="16.5" thickBot="1">
       <c r="A2" s="82"/>
       <c r="B2" s="83"/>
       <c r="C2" s="83"/>
@@ -26226,7 +26226,7 @@
       <c r="I8" s="28"/>
       <c r="J8" s="26"/>
     </row>
-    <row r="9" spans="1:16" ht="16">
+    <row r="9" spans="1:16" ht="15.75">
       <c r="A9" s="508" t="s">
         <v>336</v>
       </c>

</xml_diff>